<commit_message>
autogen UI with chartInfo
</commit_message>
<xml_diff>
--- a/inst/epivis_shiny/data_dictionaries/charts_and_enhancements.xlsx
+++ b/inst/epivis_shiny/data_dictionaries/charts_and_enhancements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acrisan/Projects/epivis/inst/epivis_shiny/data_dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F615FF-85AB-2D4B-9FAD-C5DF3824755D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F93EA5-3D97-AE47-A19F-FA85A5292F6A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{A9B4CD7A-2863-DC46-9B87-04BB3FD6856D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="28">
   <si>
     <t>chartType</t>
   </si>
@@ -50,18 +50,12 @@
     <t>size</t>
   </si>
   <si>
-    <t>hist</t>
-  </si>
-  <si>
     <t>pdf</t>
   </si>
   <si>
     <t>phyloTree</t>
   </si>
   <si>
-    <t>dendrogram</t>
-  </si>
-  <si>
     <t>map</t>
   </si>
   <si>
@@ -71,25 +65,55 @@
     <t>shape</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>point;line</t>
   </si>
   <si>
     <t>point</t>
   </si>
   <si>
-    <t>density</t>
-  </si>
-  <si>
-    <t>point;shape</t>
-  </si>
-  <si>
     <t>network</t>
+  </si>
+  <si>
+    <t>histogram</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>dataType</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>spatial</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>epicurve</t>
+  </si>
+  <si>
+    <t>xpos</t>
+  </si>
+  <si>
+    <t>ypos</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>tableRequired</t>
+  </si>
+  <si>
+    <t>dendroTree</t>
+  </si>
+  <si>
+    <t>visVars</t>
   </si>
 </sst>
 </file>
@@ -441,195 +465,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53DFF759-BE8A-1E4E-AC9C-14B2052D8BD0}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve entity graph, make console commands
</commit_message>
<xml_diff>
--- a/inst/epivis_shiny/data_dictionaries/charts_and_enhancements.xlsx
+++ b/inst/epivis_shiny/data_dictionaries/charts_and_enhancements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acrisan/Projects/epivis/inst/epivis_shiny/data_dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227E265D-19FC-164A-BEFC-1D865F528DC3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82EE1D6-EB95-4649-8CD8-3BC090E14A61}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{A9B4CD7A-2863-DC46-9B87-04BB3FD6856D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="29">
   <si>
     <t>chartType</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>visVars</t>
+  </si>
+  <si>
+    <t>phylogenetic_tree</t>
+  </si>
+  <si>
+    <t>geo</t>
   </si>
 </sst>
 </file>
@@ -465,7 +471,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,7 +656,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -720,7 +726,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>

</xml_diff>